<commit_message>
Allow bandpass filters starting at 0
Change the bandpass filter frequencies attribute from "positive" to "nonnegative" to allow filters starting at 0.
</commit_message>
<xml_diff>
--- a/src/functional_pipeline/functionalParameterProperties.xlsx
+++ b/src/functional_pipeline/functionalParameterProperties.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Documents/projects/connectomizer_develop/CATO_REBORN/CATO-utils/CATO/src/functional_pipeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/GitHub/CATO_public/src/functional_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D4EE8D-656F-2546-8D10-834AFB98C4BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC42BDFC-3723-A14A-A2C5-83953AF81FC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29220" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -297,9 +297,6 @@
     <t>functional_pipeline</t>
   </si>
   <si>
-    <t>nonempty positive</t>
-  </si>
-  <si>
     <t>scalar nonempty integer nonnegative</t>
   </si>
   <si>
@@ -439,6 +436,9 @@
   </si>
   <si>
     <t>Reference file to which fMRI data is registered</t>
+  </si>
+  <si>
+    <t>nonempty nonnegative</t>
   </si>
 </sst>
 </file>
@@ -804,7 +804,7 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -813,7 +813,7 @@
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="5.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -837,10 +837,10 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -857,10 +857,10 @@
         <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -877,15 +877,15 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
         <v>89</v>
@@ -897,15 +897,15 @@
         <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
         <v>89</v>
@@ -917,15 +917,15 @@
         <v>4</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>89</v>
@@ -937,10 +937,10 @@
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -957,10 +957,10 @@
         <v>4</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -977,10 +977,10 @@
         <v>4</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -997,10 +997,10 @@
         <v>4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1017,7 +1017,7 @@
         <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
@@ -1037,7 +1037,7 @@
         <v>31</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H11" t="s">
         <v>36</v>
@@ -1057,10 +1057,10 @@
         <v>30</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1077,10 +1077,10 @@
         <v>31</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1097,10 +1097,10 @@
         <v>31</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1117,7 +1117,7 @@
         <v>31</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H15" t="s">
         <v>37</v>
@@ -1125,24 +1125,24 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
         <v>82</v>
@@ -1151,27 +1151,27 @@
         <v>29</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1188,10 +1188,10 @@
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1208,7 +1208,7 @@
         <v>31</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H20" t="s">
         <v>66</v>
@@ -1219,7 +1219,7 @@
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
         <v>84</v>
@@ -1231,7 +1231,7 @@
         <v>31</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H21" t="s">
         <v>67</v>
@@ -1242,7 +1242,7 @@
         <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
         <v>84</v>
@@ -1254,15 +1254,15 @@
         <v>31</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -1277,10 +1277,10 @@
         <v>31</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1300,10 +1300,10 @@
         <v>31</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1311,7 +1311,7 @@
         <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
         <v>84</v>
@@ -1323,10 +1323,10 @@
         <v>31</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1343,7 +1343,7 @@
         <v>4</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H26" t="s">
         <v>68</v>
@@ -1360,10 +1360,10 @@
         <v>3</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1380,7 +1380,7 @@
         <v>31</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H28" t="s">
         <v>69</v>
@@ -1388,7 +1388,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D29" t="s">
         <v>19</v>
@@ -1397,10 +1397,10 @@
         <v>86</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1420,10 +1420,10 @@
         <v>31</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1440,10 +1440,10 @@
         <v>31</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1463,7 +1463,7 @@
         <v>31</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H32" t="s">
         <v>39</v>
@@ -1486,7 +1486,7 @@
         <v>31</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H33" t="s">
         <v>38</v>
@@ -1506,7 +1506,7 @@
         <v>31</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H34" t="s">
         <v>40</v>
@@ -1526,10 +1526,10 @@
         <v>31</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1546,10 +1546,10 @@
         <v>31</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1569,10 +1569,10 @@
         <v>31</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1589,10 +1589,10 @@
         <v>4</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1609,10 +1609,10 @@
         <v>31</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1629,10 +1629,10 @@
         <v>31</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1649,10 +1649,10 @@
         <v>87</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1669,10 +1669,10 @@
         <v>4</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1686,7 +1686,7 @@
         <v>86</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H43" t="s">
         <v>70</v>
@@ -1703,7 +1703,7 @@
         <v>86</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H44" t="s">
         <v>71</v>
@@ -1720,10 +1720,10 @@
         <v>2</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H45" t="s">
         <v>72</v>
@@ -1740,7 +1740,7 @@
         <v>86</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H46" t="s">
         <v>73</v>
@@ -1760,7 +1760,7 @@
         <v>87</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H47" t="s">
         <v>74</v>
@@ -1780,7 +1780,7 @@
         <v>87</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H48" t="s">
         <v>75</v>
@@ -1800,7 +1800,7 @@
         <v>88</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H49" t="s">
         <v>76</v>
@@ -1817,10 +1817,10 @@
         <v>2</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H50" t="s">
         <v>77</v>
@@ -1837,10 +1837,10 @@
         <v>2</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H51" t="s">
         <v>78</v>
@@ -1857,7 +1857,7 @@
         <v>86</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H52" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Add ROIs matching step to parcellation stage.
Fix such that the assigned ROIs in the parcellationFile matches the numbers of regions in the lookup table provided with the template. The ROIs can mismatch in case the order of the color lookup table of a template does not match the lookup table used to create the GCS file or the lookup table skips one region number.
</commit_message>
<xml_diff>
--- a/src/functional_pipeline/functionalParameterProperties.xlsx
+++ b/src/functional_pipeline/functionalParameterProperties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/GitHub/CATO_public/src/functional_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC42BDFC-3723-A14A-A2C5-83953AF81FC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBA1508-2709-AC40-8C6E-8723D5B058CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29220" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="141">
   <si>
     <t>parameter</t>
   </si>
@@ -99,9 +99,6 @@
     <t>collect_region_properties.statsSubFile</t>
   </si>
   <si>
-    <t>collect_region_properties.lutFile</t>
-  </si>
-  <si>
     <t>collect_region_properties.regionPropertiesFile</t>
   </si>
   <si>
@@ -439,6 +436,18 @@
   </si>
   <si>
     <t>nonempty nonnegative</t>
+  </si>
+  <si>
+    <t>parcellation.matchROIs</t>
+  </si>
+  <si>
+    <t>Flag whether the parcellation step should reassign the ROIs in the parcellationFile to match the template's color lookup table.</t>
+  </si>
+  <si>
+    <t>parcellation.lutFile</t>
+  </si>
+  <si>
+    <t>parcellation,collect_region_properties</t>
   </si>
 </sst>
 </file>
@@ -801,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601D286D-EE53-F94C-94B6-2BBF9957A3E8}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -819,13 +828,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -837,10 +846,10 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -848,19 +857,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -868,27 +877,27 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -897,18 +906,18 @@
         <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -917,18 +926,18 @@
         <v>4</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
@@ -937,10 +946,10 @@
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -948,19 +957,19 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -968,19 +977,19 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -991,16 +1000,16 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1008,19 +1017,19 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1028,19 +1037,19 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1048,19 +1057,19 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1068,19 +1077,19 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1088,19 +1097,19 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1108,78 +1117,78 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" t="s">
         <v>97</v>
-      </c>
-      <c r="D17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H17" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
         <v>3</v>
@@ -1188,242 +1197,242 @@
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
         <v>3</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E24" t="s">
         <v>3</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" t="s">
         <v>3</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
         <v>3</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E28" t="s">
         <v>3</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" t="s">
         <v>19</v>
       </c>
       <c r="E29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
         <v>19</v>
       </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1434,433 +1443,450 @@
         <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" t="s">
         <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H32" t="s">
-        <v>39</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>139</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H33" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
         <v>18</v>
       </c>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
       <c r="E34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
         <v>18</v>
       </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H35" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" t="s">
         <v>18</v>
       </c>
       <c r="E36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H36" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H37" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" t="s">
-        <v>82</v>
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
       </c>
       <c r="E38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H38" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" t="s">
-        <v>82</v>
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>81</v>
       </c>
       <c r="E39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H40" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>54</v>
-      </c>
-      <c r="D41" t="s">
-        <v>82</v>
+        <v>52</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
       </c>
       <c r="E41" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="G41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H41" t="s">
         <v>133</v>
-      </c>
-      <c r="H41" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E42" t="s">
         <v>2</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="H42" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E43" t="s">
-        <v>86</v>
+        <v>2</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H43" t="s">
-        <v>70</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E45" t="s">
-        <v>2</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H45" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E46" t="s">
-        <v>86</v>
+        <v>2</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H46" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E47" t="s">
-        <v>2</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H47" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E48" t="s">
         <v>2</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E49" t="s">
         <v>2</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H49" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E50" t="s">
         <v>2</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H50" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E51" t="s">
         <v>2</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H51" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E52" t="s">
-        <v>86</v>
+        <v>2</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H52" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="D53" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" t="s">
+        <v>85</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H53" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use lutFile parameter in functional network reconstruction step.
Use the lutFile parameter to find the color lookup table file instead of using a hard-coded file path.
</commit_message>
<xml_diff>
--- a/src/functional_pipeline/functionalParameterProperties.xlsx
+++ b/src/functional_pipeline/functionalParameterProperties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/GitHub/CATO_public/src/functional_pipeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/projects/connectomizer_develop/CATO_public/src/functional_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBA1508-2709-AC40-8C6E-8723D5B058CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF81113E-932F-BB47-BA4D-A28139ACE526}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="28700" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
     <t>parcellation.lutFile</t>
   </si>
   <si>
-    <t>parcellation,collect_region_properties</t>
+    <t>parcellation,collect_region_properties,reconstruction_functional_network</t>
   </si>
 </sst>
 </file>
@@ -813,7 +813,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add limitation on number of used computation threads
MATLAB can utilize multiple threads in some functions. At default, the maximum number of computational threads is set to the number of physical cores. The new parameter general.maxNumberCompThreads limits the number of threads which is useful when running multiple instances of CATO in parallel on clusters. If the parameter is set to 0, CATO will use the automatic value chosen by MATLAB
</commit_message>
<xml_diff>
--- a/src/functional_pipeline/functionalParameterProperties.xlsx
+++ b/src/functional_pipeline/functionalParameterProperties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/projects/connectomizer_develop/CATO_public/src/functional_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF81113E-932F-BB47-BA4D-A28139ACE526}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE072DF-B0FB-634C-A77F-7BB10D49C727}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="28700" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="145">
   <si>
     <t>parameter</t>
   </si>
@@ -448,6 +448,18 @@
   </si>
   <si>
     <t>parcellation,collect_region_properties,reconstruction_functional_network</t>
+  </si>
+  <si>
+    <t>general.maxNumberCompThreads</t>
+  </si>
+  <si>
+    <t>structural_pipeline</t>
+  </si>
+  <si>
+    <t>scalar nonempty nonnegative</t>
+  </si>
+  <si>
+    <t>Maximum number of computational threads used in pipeline. Value 0 lets MATLAB determine the most desirable number of computational threads (equal to the number of physical cores on the machine).</t>
   </si>
 </sst>
 </file>
@@ -810,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601D286D-EE53-F94C-94B6-2BBF9957A3E8}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1168,69 +1180,66 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="E18" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H18" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="E19" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G19" s="1" t="s">
         <v>101</v>
       </c>
       <c r="H19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" t="s">
-        <v>83</v>
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
       </c>
       <c r="E20" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H20" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" t="s">
         <v>83</v>
       </c>
       <c r="E21" t="s">
@@ -1243,12 +1252,12 @@
         <v>100</v>
       </c>
       <c r="H21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>91</v>
@@ -1266,15 +1275,15 @@
         <v>100</v>
       </c>
       <c r="H22" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
         <v>83</v>
@@ -1289,12 +1298,12 @@
         <v>100</v>
       </c>
       <c r="H23" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
@@ -1312,15 +1321,15 @@
         <v>100</v>
       </c>
       <c r="H24" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
         <v>83</v>
@@ -1335,111 +1344,114 @@
         <v>100</v>
       </c>
       <c r="H25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" t="s">
         <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H26" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
         <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>85</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>122</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" t="s">
         <v>83</v>
       </c>
       <c r="E28" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G28" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H28" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" t="s">
-        <v>19</v>
+        <v>48</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>3</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H29" t="s">
-        <v>123</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" t="s">
         <v>19</v>
       </c>
       <c r="E30" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
         <v>19</v>
       </c>
       <c r="E31" t="s">
@@ -1452,55 +1464,52 @@
         <v>100</v>
       </c>
       <c r="H31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>137</v>
-      </c>
-      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
         <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>27</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H32" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>139</v>
-      </c>
-      <c r="B33" t="s">
-        <v>140</v>
+        <v>137</v>
+      </c>
+      <c r="D33" t="s">
+        <v>19</v>
       </c>
       <c r="E33" t="s">
-        <v>27</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H33" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="E34" t="s">
         <v>27</v>
@@ -1512,12 +1521,12 @@
         <v>100</v>
       </c>
       <c r="H34" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
         <v>18</v>
@@ -1535,16 +1544,19 @@
         <v>100</v>
       </c>
       <c r="H35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
         <v>18</v>
       </c>
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
       <c r="E36" t="s">
         <v>27</v>
       </c>
@@ -1555,14 +1567,14 @@
         <v>100</v>
       </c>
       <c r="H36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
         <v>18</v>
       </c>
       <c r="E37" t="s">
@@ -1575,18 +1587,15 @@
         <v>100</v>
       </c>
       <c r="H37" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E38" t="s">
         <v>27</v>
@@ -1598,52 +1607,55 @@
         <v>100</v>
       </c>
       <c r="H38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
         <v>81</v>
+      </c>
+      <c r="C39" t="s">
+        <v>84</v>
       </c>
       <c r="E39" t="s">
         <v>27</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" t="s">
         <v>81</v>
       </c>
       <c r="E40" t="s">
         <v>27</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C41" t="s">
         <v>81</v>
@@ -1658,32 +1670,32 @@
         <v>100</v>
       </c>
       <c r="H41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>53</v>
-      </c>
-      <c r="D42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" t="s">
         <v>81</v>
       </c>
       <c r="E42" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="H42" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D43" t="s">
         <v>81</v>
@@ -1692,35 +1704,38 @@
         <v>2</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="H43" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D44" t="s">
         <v>81</v>
       </c>
       <c r="E44" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H44" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D45" t="s">
         <v>81</v>
@@ -1732,69 +1747,66 @@
         <v>100</v>
       </c>
       <c r="H45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D46" t="s">
         <v>81</v>
       </c>
       <c r="E46" t="s">
-        <v>2</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" t="s">
         <v>81</v>
       </c>
       <c r="E47" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D48" t="s">
         <v>81</v>
       </c>
       <c r="E48" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D49" t="s">
         <v>81</v>
@@ -1809,12 +1821,12 @@
         <v>100</v>
       </c>
       <c r="H49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D50" t="s">
         <v>81</v>
@@ -1823,18 +1835,18 @@
         <v>2</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D51" t="s">
         <v>81</v>
@@ -1843,18 +1855,18 @@
         <v>2</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D52" t="s">
         <v>81</v>
@@ -1869,23 +1881,43 @@
         <v>100</v>
       </c>
       <c r="H52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D53" t="s">
         <v>81</v>
       </c>
       <c r="E53" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" t="s">
+        <v>81</v>
+      </c>
+      <c r="E54" t="s">
         <v>85</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H53" t="s">
+      <c r="G54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H54" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add variable FC estimation method
</commit_message>
<xml_diff>
--- a/src/functional_pipeline/functionalParameterProperties.xlsx
+++ b/src/functional_pipeline/functionalParameterProperties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/projects/connectomizer_develop/CATO_public/src/functional_pipeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/GitHub/CATO_public/src/functional_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE072DF-B0FB-634C-A77F-7BB10D49C727}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB3EF7F-FD96-D541-93DB-76836067FD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="28700" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="148">
   <si>
     <t>parameter</t>
   </si>
@@ -460,6 +460,15 @@
   </si>
   <si>
     <t>Maximum number of computational threads used in pipeline. Value 0 lets MATLAB determine the most desirable number of computational threads (equal to the number of physical cores on the machine).</t>
+  </si>
+  <si>
+    <t>reconstruction_functional_network.reconstructionMethod</t>
+  </si>
+  <si>
+    <t>Functional connectivity estimation method used.</t>
+  </si>
+  <si>
+    <t>isfunction nonempty</t>
   </si>
 </sst>
 </file>
@@ -822,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601D286D-EE53-F94C-94B6-2BBF9957A3E8}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1655,27 +1664,27 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" t="s">
         <v>81</v>
       </c>
       <c r="E41" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H41" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
         <v>81</v>
@@ -1690,32 +1699,32 @@
         <v>100</v>
       </c>
       <c r="H42" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" t="s">
         <v>81</v>
       </c>
       <c r="E43" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="H43" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D44" t="s">
         <v>81</v>
@@ -1724,35 +1733,38 @@
         <v>2</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="H44" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
         <v>81</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H45" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
         <v>81</v>
@@ -1764,69 +1776,66 @@
         <v>100</v>
       </c>
       <c r="H46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D47" t="s">
         <v>81</v>
       </c>
       <c r="E47" t="s">
-        <v>2</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D48" t="s">
         <v>81</v>
       </c>
       <c r="E48" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D49" t="s">
         <v>81</v>
       </c>
       <c r="E49" t="s">
-        <v>2</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D50" t="s">
         <v>81</v>
@@ -1841,12 +1850,12 @@
         <v>100</v>
       </c>
       <c r="H50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D51" t="s">
         <v>81</v>
@@ -1855,18 +1864,18 @@
         <v>2</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D52" t="s">
         <v>81</v>
@@ -1875,18 +1884,18 @@
         <v>2</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D53" t="s">
         <v>81</v>
@@ -1901,23 +1910,43 @@
         <v>100</v>
       </c>
       <c r="H53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D54" t="s">
         <v>81</v>
       </c>
       <c r="E54" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" t="s">
         <v>85</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H54" t="s">
+      <c r="G55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H55" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Partial correlation feature (#10)
Let the user define the functional connectivity estimation method. This added one parameter to the configuration file ("reconstructionMethod", in line with SC pipeline). The default estimation method remains "corr" and the default behavior of the pipeline does not change.
</commit_message>
<xml_diff>
--- a/src/functional_pipeline/functionalParameterProperties.xlsx
+++ b/src/functional_pipeline/functionalParameterProperties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/projects/connectomizer_develop/CATO_public/src/functional_pipeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/GitHub/CATO_public/src/functional_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE072DF-B0FB-634C-A77F-7BB10D49C727}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB3EF7F-FD96-D541-93DB-76836067FD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="28700" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="148">
   <si>
     <t>parameter</t>
   </si>
@@ -460,6 +460,15 @@
   </si>
   <si>
     <t>Maximum number of computational threads used in pipeline. Value 0 lets MATLAB determine the most desirable number of computational threads (equal to the number of physical cores on the machine).</t>
+  </si>
+  <si>
+    <t>reconstruction_functional_network.reconstructionMethod</t>
+  </si>
+  <si>
+    <t>Functional connectivity estimation method used.</t>
+  </si>
+  <si>
+    <t>isfunction nonempty</t>
   </si>
 </sst>
 </file>
@@ -822,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601D286D-EE53-F94C-94B6-2BBF9957A3E8}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1655,27 +1664,27 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" t="s">
         <v>81</v>
       </c>
       <c r="E41" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H41" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
         <v>81</v>
@@ -1690,32 +1699,32 @@
         <v>100</v>
       </c>
       <c r="H42" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" t="s">
         <v>81</v>
       </c>
       <c r="E43" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="H43" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D44" t="s">
         <v>81</v>
@@ -1724,35 +1733,38 @@
         <v>2</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="H44" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
         <v>81</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H45" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
         <v>81</v>
@@ -1764,69 +1776,66 @@
         <v>100</v>
       </c>
       <c r="H46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D47" t="s">
         <v>81</v>
       </c>
       <c r="E47" t="s">
-        <v>2</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D48" t="s">
         <v>81</v>
       </c>
       <c r="E48" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D49" t="s">
         <v>81</v>
       </c>
       <c r="E49" t="s">
-        <v>2</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D50" t="s">
         <v>81</v>
@@ -1841,12 +1850,12 @@
         <v>100</v>
       </c>
       <c r="H50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D51" t="s">
         <v>81</v>
@@ -1855,18 +1864,18 @@
         <v>2</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D52" t="s">
         <v>81</v>
@@ -1875,18 +1884,18 @@
         <v>2</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D53" t="s">
         <v>81</v>
@@ -1901,23 +1910,43 @@
         <v>100</v>
       </c>
       <c r="H53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D54" t="s">
         <v>81</v>
       </c>
       <c r="E54" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" t="s">
         <v>85</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H54" t="s">
+      <c r="G55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H55" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add mri_convertOptions as standard parameter
</commit_message>
<xml_diff>
--- a/src/functional_pipeline/functionalParameterProperties.xlsx
+++ b/src/functional_pipeline/functionalParameterProperties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/GitHub/CATO_public/src/functional_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB3EF7F-FD96-D541-93DB-76836067FD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50DB9DC-0179-3247-B571-7CD6054D63E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="150">
   <si>
     <t>parameter</t>
   </si>
@@ -469,6 +469,12 @@
   </si>
   <si>
     <t>isfunction nonempty</t>
+  </si>
+  <si>
+    <t>functional_preprocessing.mri_convertOptions</t>
+  </si>
+  <si>
+    <t>Adjust variables in the fmriProcessedFile header (using mri_convert). Options are provided as structure (e.g. mri_convertOptions:{"tr": TR in msec, "te": TE in msec}). If emtpy, header is not changed.</t>
   </si>
 </sst>
 </file>
@@ -831,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601D286D-EE53-F94C-94B6-2BBF9957A3E8}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1418,69 +1424,66 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29" t="s">
         <v>83</v>
       </c>
       <c r="E29" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G29" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H29" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" t="s">
-        <v>19</v>
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>3</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H30" t="s">
-        <v>123</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
         <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" t="s">
         <v>19</v>
       </c>
       <c r="E32" t="s">
@@ -1493,55 +1496,52 @@
         <v>100</v>
       </c>
       <c r="H32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>137</v>
-      </c>
-      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
         <v>19</v>
       </c>
       <c r="E33" t="s">
-        <v>85</v>
+        <v>27</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H33" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>139</v>
-      </c>
-      <c r="B34" t="s">
-        <v>140</v>
+        <v>137</v>
+      </c>
+      <c r="D34" t="s">
+        <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H34" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="E35" t="s">
         <v>27</v>
@@ -1553,12 +1553,12 @@
         <v>100</v>
       </c>
       <c r="H35" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
         <v>18</v>
@@ -1576,16 +1576,19 @@
         <v>100</v>
       </c>
       <c r="H36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
         <v>18</v>
       </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
       <c r="E37" t="s">
         <v>27</v>
       </c>
@@ -1596,14 +1599,14 @@
         <v>100</v>
       </c>
       <c r="H37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
         <v>18</v>
       </c>
       <c r="E38" t="s">
@@ -1616,18 +1619,15 @@
         <v>100</v>
       </c>
       <c r="H38" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E39" t="s">
         <v>27</v>
@@ -1639,72 +1639,75 @@
         <v>100</v>
       </c>
       <c r="H39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" t="s">
         <v>81</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
       </c>
       <c r="E40" t="s">
         <v>27</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>50</v>
       </c>
       <c r="D41" t="s">
         <v>81</v>
       </c>
       <c r="E41" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>147</v>
+        <v>4</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H41" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" t="s">
         <v>81</v>
       </c>
       <c r="E42" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H42" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
         <v>81</v>
@@ -1719,32 +1722,32 @@
         <v>100</v>
       </c>
       <c r="H43" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s">
         <v>81</v>
       </c>
       <c r="E44" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="H44" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D45" t="s">
         <v>81</v>
@@ -1753,35 +1756,38 @@
         <v>2</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="H45" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D46" t="s">
         <v>81</v>
       </c>
       <c r="E46" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H46" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D47" t="s">
         <v>81</v>
@@ -1793,69 +1799,66 @@
         <v>100</v>
       </c>
       <c r="H47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D48" t="s">
         <v>81</v>
       </c>
       <c r="E48" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D49" t="s">
         <v>81</v>
       </c>
       <c r="E49" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D50" t="s">
         <v>81</v>
       </c>
       <c r="E50" t="s">
-        <v>2</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D51" t="s">
         <v>81</v>
@@ -1870,12 +1873,12 @@
         <v>100</v>
       </c>
       <c r="H51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D52" t="s">
         <v>81</v>
@@ -1884,18 +1887,18 @@
         <v>2</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
         <v>81</v>
@@ -1904,18 +1907,18 @@
         <v>2</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D54" t="s">
         <v>81</v>
@@ -1930,23 +1933,43 @@
         <v>100</v>
       </c>
       <c r="H54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D55" t="s">
         <v>81</v>
       </c>
       <c r="E55" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" t="s">
+        <v>81</v>
+      </c>
+      <c r="E56" t="s">
         <v>85</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H55" t="s">
+      <c r="G56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H56" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rename mri_convertOptions to fmriInfo
Naming the parameter `fmriInfo` makes the parameter method agnostic. This makes it easier to adjust the method in the future (e.g. implement it in MATLAB). Further it is more in line with other parameters that focus on the aim and not on the method underlying the parameter.
</commit_message>
<xml_diff>
--- a/src/functional_pipeline/functionalParameterProperties.xlsx
+++ b/src/functional_pipeline/functionalParameterProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/GitHub/CATO_public/src/functional_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50DB9DC-0179-3247-B571-7CD6054D63E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5162C6B5-53DD-4444-957C-735457241BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
@@ -471,10 +471,10 @@
     <t>isfunction nonempty</t>
   </si>
   <si>
-    <t>functional_preprocessing.mri_convertOptions</t>
-  </si>
-  <si>
-    <t>Adjust variables in the fmriProcessedFile header (using mri_convert). Options are provided as structure (e.g. mri_convertOptions:{"tr": TR in msec, "te": TE in msec}). If emtpy, header is not changed.</t>
+    <t>functional_preprocessing.fmriInfo</t>
+  </si>
+  <si>
+    <t>Adjust variables in the fmriProcessedFile header (using mri_convert). Options are provided as structure (e.g. fmriInfo:{"tr": TR in msec, "te": TE in msec}). If emtpy, header is not changed.</t>
   </si>
 </sst>
 </file>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601D286D-EE53-F94C-94B6-2BBF9957A3E8}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add check on TR in default functional preprocessing script (#21)
Add an option to the preprocessing script to adjust the rs-fMRI NIfTI header (using mri_convert from FreeSurfer). This functionality can be used to the repetition time. Furthermore, add a check in the default functional preprocessing script to ensure that the repetition time is non-zero (not missing).
</commit_message>
<xml_diff>
--- a/src/functional_pipeline/functionalParameterProperties.xlsx
+++ b/src/functional_pipeline/functionalParameterProperties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/GitHub/CATO_public/src/functional_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB3EF7F-FD96-D541-93DB-76836067FD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5162C6B5-53DD-4444-957C-735457241BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="150">
   <si>
     <t>parameter</t>
   </si>
@@ -469,6 +469,12 @@
   </si>
   <si>
     <t>isfunction nonempty</t>
+  </si>
+  <si>
+    <t>functional_preprocessing.fmriInfo</t>
+  </si>
+  <si>
+    <t>Adjust variables in the fmriProcessedFile header (using mri_convert). Options are provided as structure (e.g. fmriInfo:{"tr": TR in msec, "te": TE in msec}). If emtpy, header is not changed.</t>
   </si>
 </sst>
 </file>
@@ -831,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601D286D-EE53-F94C-94B6-2BBF9957A3E8}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1418,69 +1424,66 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29" t="s">
         <v>83</v>
       </c>
       <c r="E29" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G29" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H29" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" t="s">
-        <v>19</v>
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>3</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H30" t="s">
-        <v>123</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
         <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" t="s">
         <v>19</v>
       </c>
       <c r="E32" t="s">
@@ -1493,55 +1496,52 @@
         <v>100</v>
       </c>
       <c r="H32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>137</v>
-      </c>
-      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
         <v>19</v>
       </c>
       <c r="E33" t="s">
-        <v>85</v>
+        <v>27</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H33" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>139</v>
-      </c>
-      <c r="B34" t="s">
-        <v>140</v>
+        <v>137</v>
+      </c>
+      <c r="D34" t="s">
+        <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H34" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="E35" t="s">
         <v>27</v>
@@ -1553,12 +1553,12 @@
         <v>100</v>
       </c>
       <c r="H35" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
         <v>18</v>
@@ -1576,16 +1576,19 @@
         <v>100</v>
       </c>
       <c r="H36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
         <v>18</v>
       </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
       <c r="E37" t="s">
         <v>27</v>
       </c>
@@ -1596,14 +1599,14 @@
         <v>100</v>
       </c>
       <c r="H37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
         <v>18</v>
       </c>
       <c r="E38" t="s">
@@ -1616,18 +1619,15 @@
         <v>100</v>
       </c>
       <c r="H38" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E39" t="s">
         <v>27</v>
@@ -1639,72 +1639,75 @@
         <v>100</v>
       </c>
       <c r="H39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" t="s">
         <v>81</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
       </c>
       <c r="E40" t="s">
         <v>27</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>50</v>
       </c>
       <c r="D41" t="s">
         <v>81</v>
       </c>
       <c r="E41" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>147</v>
+        <v>4</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H41" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" t="s">
         <v>81</v>
       </c>
       <c r="E42" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H42" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
         <v>81</v>
@@ -1719,32 +1722,32 @@
         <v>100</v>
       </c>
       <c r="H43" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s">
         <v>81</v>
       </c>
       <c r="E44" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="H44" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D45" t="s">
         <v>81</v>
@@ -1753,35 +1756,38 @@
         <v>2</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="H45" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D46" t="s">
         <v>81</v>
       </c>
       <c r="E46" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H46" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D47" t="s">
         <v>81</v>
@@ -1793,69 +1799,66 @@
         <v>100</v>
       </c>
       <c r="H47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D48" t="s">
         <v>81</v>
       </c>
       <c r="E48" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D49" t="s">
         <v>81</v>
       </c>
       <c r="E49" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D50" t="s">
         <v>81</v>
       </c>
       <c r="E50" t="s">
-        <v>2</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D51" t="s">
         <v>81</v>
@@ -1870,12 +1873,12 @@
         <v>100</v>
       </c>
       <c r="H51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D52" t="s">
         <v>81</v>
@@ -1884,18 +1887,18 @@
         <v>2</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
         <v>81</v>
@@ -1904,18 +1907,18 @@
         <v>2</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D54" t="s">
         <v>81</v>
@@ -1930,23 +1933,43 @@
         <v>100</v>
       </c>
       <c r="H54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D55" t="s">
         <v>81</v>
       </c>
       <c r="E55" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" t="s">
+        <v>81</v>
+      </c>
+      <c r="E56" t="s">
         <v>85</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H55" t="s">
+      <c r="G56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H56" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add option to truncate timeseries
</commit_message>
<xml_diff>
--- a/src/functional_pipeline/functionalParameterProperties.xlsx
+++ b/src/functional_pipeline/functionalParameterProperties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/GitHub/CATO_public/src/functional_pipeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koen/sw/CATO/src/functional_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5162C6B5-53DD-4444-957C-735457241BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480B9DB8-7677-4047-8EED-6506CC3C361A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
+    <workbookView xWindow="1260" yWindow="760" windowWidth="28800" windowHeight="18000" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="152">
   <si>
     <t>parameter</t>
   </si>
@@ -475,6 +475,12 @@
   </si>
   <si>
     <t>Adjust variables in the fmriProcessedFile header (using mri_convert). Options are provided as structure (e.g. fmriInfo:{"tr": TR in msec, "te": TE in msec}). If emtpy, header is not changed.</t>
+  </si>
+  <si>
+    <t>reconstruction_functional_network.truncateFrames</t>
+  </si>
+  <si>
+    <t>Number of frames at beginning and end of timeseries to always remove</t>
   </si>
 </sst>
 </file>
@@ -837,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601D286D-EE53-F94C-94B6-2BBF9957A3E8}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1841,44 +1847,44 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>150</v>
       </c>
       <c r="D50" t="s">
         <v>81</v>
       </c>
       <c r="E50" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H50" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D51" t="s">
         <v>81</v>
       </c>
       <c r="E51" t="s">
-        <v>2</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D52" t="s">
         <v>81</v>
@@ -1893,12 +1899,12 @@
         <v>100</v>
       </c>
       <c r="H52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D53" t="s">
         <v>81</v>
@@ -1907,18 +1913,18 @@
         <v>2</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D54" t="s">
         <v>81</v>
@@ -1927,18 +1933,18 @@
         <v>2</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D55" t="s">
         <v>81</v>
@@ -1953,23 +1959,43 @@
         <v>100</v>
       </c>
       <c r="H55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D56" t="s">
         <v>81</v>
       </c>
       <c r="E56" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" t="s">
+        <v>81</v>
+      </c>
+      <c r="E57" t="s">
         <v>85</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H56" t="s">
+      <c r="G57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H57" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>